<commit_message>
Updates for tool paper
updates to figures and module eff. Bonus csv of installs by state since 2010
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/Harmonize_graphs.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/Harmonize_graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56411CA-0E79-4496-8F7A-9E7590494832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FAACFF-193F-4168-AF00-B8B4070DEF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D931EBBB-F0C0-4C12-9066-9D55B5844573}"/>
+    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{D931EBBB-F0C0-4C12-9066-9D55B5844573}"/>
   </bookViews>
   <sheets>
     <sheet name="USInstallsLitCompare" sheetId="1" r:id="rId1"/>
@@ -209,9 +209,6 @@
     <t>M. Bolinger et al 2019 "utility scale"</t>
   </si>
   <si>
-    <t>PV ICE Si-only Annual Installs</t>
-  </si>
-  <si>
     <t>Wood Mackenzie US PV Forecasts Report - 2020-yir</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>ton/MW</t>
+  </si>
+  <si>
+    <t>Baseline</t>
   </si>
 </sst>
 </file>
@@ -2228,7 +2228,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PV ICE Si-only Annual Installs</c:v>
+                  <c:v>Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2771,12 +2771,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -27546,11 +27541,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61314F7D-DD79-469D-B970-9A7E66501C25}">
   <dimension ref="A1:AK1014"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AS21" sqref="AS21"/>
+      <selection pane="bottomRight" activeCell="AA45" sqref="AA45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27575,13 +27570,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>52</v>
@@ -52731,7 +52726,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="40"/>
       <c r="D1" s="40"/>
@@ -53843,7 +53838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A705CA4-15CE-47FA-BD3E-74BB8D3BD66C}">
   <dimension ref="A1:AI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -53866,22 +53861,22 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B1" s="40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="40"/>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>61</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>62</v>
       </c>
       <c r="I1" s="33"/>
       <c r="J1" s="34"/>
       <c r="K1" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="33"/>
       <c r="M1" s="33"/>
@@ -53901,17 +53896,17 @@
       <c r="AA1" s="33"/>
       <c r="AB1" s="33"/>
       <c r="AC1" s="40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD1" s="40"/>
       <c r="AE1" s="40"/>
       <c r="AF1" s="40"/>
       <c r="AG1" s="40"/>
       <c r="AH1" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI1" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="AI1" s="36" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
@@ -53919,76 +53914,76 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>72</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>73</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>74</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>75</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>76</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>78</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>79</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>81</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>82</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AC2" t="s">
         <v>83</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>84</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>85</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>86</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>87</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" t="s">
         <v>88</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">

</xml_diff>